<commit_message>
Add detail for previous year. Fix mistake in date references. Add docstrings.
</commit_message>
<xml_diff>
--- a/sample_finances.xlsx
+++ b/sample_finances.xlsx
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="110" uniqueCount="56">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="110" uniqueCount="54">
   <si>
     <t>Item</t>
   </si>
@@ -59,15 +59,9 @@
     <t>ATM w/drawal</t>
   </si>
   <si>
-    <t>Verizon</t>
-  </si>
-  <si>
     <t>MD Estimated Tax</t>
   </si>
   <si>
-    <t>CarMax Auto Finance</t>
-  </si>
-  <si>
     <t>ATM withdrawal</t>
   </si>
   <si>
@@ -77,30 +71,12 @@
     <t>Rent</t>
   </si>
   <si>
-    <t>Verizon Autodebit</t>
-  </si>
-  <si>
     <t>partial Rent</t>
   </si>
   <si>
-    <t>Pepco</t>
-  </si>
-  <si>
-    <t>Washington Gas</t>
-  </si>
-  <si>
-    <t>Sprint</t>
-  </si>
-  <si>
-    <t>ATM withdrawal - Chevy Chase</t>
-  </si>
-  <si>
     <t>fee for ATM withdrawal</t>
   </si>
   <si>
-    <t>Sprint (incl. overdue payment)</t>
-  </si>
-  <si>
     <t>LabCorp</t>
   </si>
   <si>
@@ -116,9 +92,6 @@
     <t>Check printing charge</t>
   </si>
   <si>
-    <t>American Mutual Fund Autodebit</t>
-  </si>
-  <si>
     <t>Wire Transfer fee</t>
   </si>
   <si>
@@ -195,6 +168,27 @@
   </si>
   <si>
     <t>Exelon Gas</t>
+  </si>
+  <si>
+    <t>Car rental</t>
+  </si>
+  <si>
+    <t>Cell phone</t>
+  </si>
+  <si>
+    <t>Landline automatic payment</t>
+  </si>
+  <si>
+    <t>cell phone (incl. overdue payment)</t>
+  </si>
+  <si>
+    <t>Landline</t>
+  </si>
+  <si>
+    <t>Gas bill</t>
+  </si>
+  <si>
+    <t>Auto Finance</t>
   </si>
 </sst>
 </file>
@@ -612,8 +606,8 @@
   <dimension ref="A1:G129"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="3" topLeftCell="A44" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C98" sqref="C98"/>
+      <pane ySplit="3" topLeftCell="A18" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="C41" sqref="C41"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.7109375" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -631,7 +625,7 @@
   <sheetData>
     <row r="1" spans="1:7" s="5" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A1" s="8" t="s">
-        <v>32</v>
+        <v>23</v>
       </c>
       <c r="B1" s="4"/>
       <c r="C1" s="9"/>
@@ -642,7 +636,7 @@
     </row>
     <row r="2" spans="1:7" s="5" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A2" s="9" t="s">
-        <v>33</v>
+        <v>24</v>
       </c>
       <c r="B2" s="4"/>
       <c r="C2" s="9"/>
@@ -688,7 +682,7 @@
         <v>38806</v>
       </c>
       <c r="C5" s="5" t="s">
-        <v>34</v>
+        <v>25</v>
       </c>
       <c r="D5" s="6"/>
       <c r="E5" s="6">
@@ -728,7 +722,7 @@
         <v>38834</v>
       </c>
       <c r="C7" s="5" t="s">
-        <v>34</v>
+        <v>25</v>
       </c>
       <c r="D7" s="6"/>
       <c r="E7" s="6">
@@ -771,7 +765,7 @@
         <v>38859</v>
       </c>
       <c r="C9" s="5" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="D9" s="6">
         <v>1413</v>
@@ -814,7 +808,7 @@
         <v>38893</v>
       </c>
       <c r="C11" s="5" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="D11" s="6">
         <v>1134</v>
@@ -834,7 +828,7 @@
         <v>38901</v>
       </c>
       <c r="C12" s="5" t="s">
-        <v>34</v>
+        <v>25</v>
       </c>
       <c r="D12" s="6"/>
       <c r="E12" s="6">
@@ -857,7 +851,7 @@
         <v>38913</v>
       </c>
       <c r="C13" s="5" t="s">
-        <v>10</v>
+        <v>51</v>
       </c>
       <c r="D13" s="6">
         <v>82.88</v>
@@ -877,7 +871,7 @@
         <v>38936</v>
       </c>
       <c r="C14" s="5" t="s">
-        <v>34</v>
+        <v>25</v>
       </c>
       <c r="D14" s="6"/>
       <c r="E14" s="6">
@@ -900,7 +894,7 @@
         <v>38942</v>
       </c>
       <c r="C15" s="5" t="s">
-        <v>35</v>
+        <v>26</v>
       </c>
       <c r="D15" s="6">
         <v>46.35</v>
@@ -920,7 +914,7 @@
         <v>38959</v>
       </c>
       <c r="C16" s="5" t="s">
-        <v>36</v>
+        <v>27</v>
       </c>
       <c r="D16" s="6"/>
       <c r="E16" s="6">
@@ -943,7 +937,7 @@
         <v>38989</v>
       </c>
       <c r="C17" s="5" t="s">
-        <v>37</v>
+        <v>28</v>
       </c>
       <c r="D17" s="6"/>
       <c r="E17" s="6">
@@ -983,7 +977,7 @@
         <v>39037</v>
       </c>
       <c r="C19" s="5" t="s">
-        <v>38</v>
+        <v>29</v>
       </c>
       <c r="D19" s="6"/>
       <c r="E19" s="6">
@@ -1006,7 +1000,7 @@
         <v>39067</v>
       </c>
       <c r="C20" s="5" t="s">
-        <v>35</v>
+        <v>26</v>
       </c>
       <c r="D20" s="6">
         <v>46.35</v>
@@ -1026,7 +1020,7 @@
         <v>39087</v>
       </c>
       <c r="C21" s="5" t="s">
-        <v>34</v>
+        <v>25</v>
       </c>
       <c r="D21" s="6"/>
       <c r="E21" s="6">
@@ -1049,7 +1043,7 @@
         <v>39094</v>
       </c>
       <c r="C22" s="5" t="s">
-        <v>35</v>
+        <v>26</v>
       </c>
       <c r="D22" s="6">
         <v>46.35</v>
@@ -1069,7 +1063,7 @@
         <v>39117</v>
       </c>
       <c r="C23" s="5" t="s">
-        <v>34</v>
+        <v>25</v>
       </c>
       <c r="D23" s="6"/>
       <c r="E23" s="6">
@@ -1092,7 +1086,7 @@
         <v>39135</v>
       </c>
       <c r="C24" s="5" t="s">
-        <v>41</v>
+        <v>32</v>
       </c>
       <c r="D24" s="6">
         <v>809.71</v>
@@ -1112,7 +1106,7 @@
         <v>39170</v>
       </c>
       <c r="C25" s="5" t="s">
-        <v>34</v>
+        <v>25</v>
       </c>
       <c r="D25" s="6"/>
       <c r="E25" s="6">
@@ -1152,7 +1146,7 @@
         <v>39190</v>
       </c>
       <c r="C27" s="5" t="s">
-        <v>34</v>
+        <v>25</v>
       </c>
       <c r="D27" s="6"/>
       <c r="E27" s="6">
@@ -1175,7 +1169,7 @@
         <v>39217</v>
       </c>
       <c r="C28" s="5" t="s">
-        <v>40</v>
+        <v>31</v>
       </c>
       <c r="D28" s="6">
         <v>478</v>
@@ -1195,7 +1189,7 @@
         <v>39232</v>
       </c>
       <c r="C29" s="5" t="s">
-        <v>34</v>
+        <v>25</v>
       </c>
       <c r="D29" s="6"/>
       <c r="E29" s="6">
@@ -1218,7 +1212,7 @@
         <v>39260</v>
       </c>
       <c r="C30" s="5" t="s">
-        <v>41</v>
+        <v>32</v>
       </c>
       <c r="D30" s="6">
         <v>868.27</v>
@@ -1238,7 +1232,7 @@
         <v>39627</v>
       </c>
       <c r="C31" s="5" t="s">
-        <v>34</v>
+        <v>25</v>
       </c>
       <c r="D31" s="6"/>
       <c r="E31" s="6">
@@ -1261,7 +1255,7 @@
         <v>39308</v>
       </c>
       <c r="C32" s="5" t="s">
-        <v>35</v>
+        <v>26</v>
       </c>
       <c r="D32" s="6">
         <v>46.35</v>
@@ -1281,7 +1275,7 @@
         <v>39318</v>
       </c>
       <c r="C33" s="5" t="s">
-        <v>34</v>
+        <v>25</v>
       </c>
       <c r="D33" s="6"/>
       <c r="E33" s="6">
@@ -1304,7 +1298,7 @@
         <v>39355</v>
       </c>
       <c r="C34" s="5" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="D34" s="6">
         <v>954</v>
@@ -1324,7 +1318,7 @@
         <v>39385</v>
       </c>
       <c r="C35" s="5" t="s">
-        <v>34</v>
+        <v>25</v>
       </c>
       <c r="D35" s="6"/>
       <c r="E35" s="6">
@@ -1347,7 +1341,7 @@
         <v>39403</v>
       </c>
       <c r="C36" s="5" t="s">
-        <v>35</v>
+        <v>26</v>
       </c>
       <c r="D36" s="6">
         <v>46.92</v>
@@ -1367,7 +1361,7 @@
         <v>39407</v>
       </c>
       <c r="C37" s="5" t="s">
-        <v>34</v>
+        <v>25</v>
       </c>
       <c r="D37" s="6"/>
       <c r="E37" s="6">
@@ -1387,7 +1381,7 @@
         <v>39410</v>
       </c>
       <c r="C38" s="5" t="s">
-        <v>28</v>
+        <v>20</v>
       </c>
       <c r="D38" s="6">
         <v>25</v>
@@ -1407,7 +1401,7 @@
         <v>39421</v>
       </c>
       <c r="C39" s="5" t="s">
-        <v>34</v>
+        <v>25</v>
       </c>
       <c r="D39" s="6"/>
       <c r="E39" s="6">
@@ -1430,7 +1424,7 @@
         <v>39442</v>
       </c>
       <c r="C40" s="7" t="s">
-        <v>12</v>
+        <v>53</v>
       </c>
       <c r="D40" s="6">
         <v>54.43</v>
@@ -1450,7 +1444,7 @@
         <v>39465</v>
       </c>
       <c r="C41" s="5" t="s">
-        <v>34</v>
+        <v>25</v>
       </c>
       <c r="D41" s="6"/>
       <c r="E41" s="6">
@@ -1473,7 +1467,7 @@
         <v>39493</v>
       </c>
       <c r="C42" s="5" t="s">
-        <v>42</v>
+        <v>33</v>
       </c>
       <c r="D42" s="6">
         <v>88.55</v>
@@ -1493,7 +1487,7 @@
         <v>39497</v>
       </c>
       <c r="C43" s="5" t="s">
-        <v>34</v>
+        <v>25</v>
       </c>
       <c r="D43" s="6"/>
       <c r="E43" s="6">
@@ -1533,7 +1527,7 @@
         <v>39565</v>
       </c>
       <c r="C45" s="5" t="s">
-        <v>34</v>
+        <v>25</v>
       </c>
       <c r="D45" s="6"/>
       <c r="E45" s="6">
@@ -1556,7 +1550,7 @@
         <v>39597</v>
       </c>
       <c r="C46" s="5" t="s">
-        <v>17</v>
+        <v>14</v>
       </c>
       <c r="D46" s="6">
         <v>495</v>
@@ -1576,7 +1570,7 @@
         <v>39617</v>
       </c>
       <c r="C47" s="5" t="s">
-        <v>34</v>
+        <v>25</v>
       </c>
       <c r="D47" s="6"/>
       <c r="E47" s="6">
@@ -1596,7 +1590,7 @@
         <v>39642</v>
       </c>
       <c r="C48" s="5" t="s">
-        <v>51</v>
+        <v>42</v>
       </c>
       <c r="D48" s="6">
         <v>20000</v>
@@ -1639,7 +1633,7 @@
         <v>39746</v>
       </c>
       <c r="C50" s="5" t="s">
-        <v>43</v>
+        <v>34</v>
       </c>
       <c r="D50" s="6">
         <v>703.13</v>
@@ -1662,7 +1656,7 @@
         <v>39810</v>
       </c>
       <c r="C51" s="5" t="s">
-        <v>49</v>
+        <v>40</v>
       </c>
       <c r="D51" s="6">
         <v>75</v>
@@ -1682,7 +1676,7 @@
         <v>39845</v>
       </c>
       <c r="C52" s="5" t="s">
-        <v>34</v>
+        <v>25</v>
       </c>
       <c r="D52" s="6"/>
       <c r="E52" s="6">
@@ -1705,7 +1699,7 @@
         <v>39875</v>
       </c>
       <c r="C53" s="5" t="s">
-        <v>44</v>
+        <v>35</v>
       </c>
       <c r="D53" s="6">
         <v>59</v>
@@ -1745,7 +1739,7 @@
         <v>39998</v>
       </c>
       <c r="C55" s="5" t="s">
-        <v>45</v>
+        <v>36</v>
       </c>
       <c r="D55" s="6"/>
       <c r="E55" s="6">
@@ -1768,7 +1762,7 @@
         <v>40067</v>
       </c>
       <c r="C56" s="5" t="s">
-        <v>39</v>
+        <v>30</v>
       </c>
       <c r="D56" s="6">
         <v>123.59</v>
@@ -1788,7 +1782,7 @@
         <v>40091</v>
       </c>
       <c r="C57" s="5" t="s">
-        <v>34</v>
+        <v>25</v>
       </c>
       <c r="D57" s="6"/>
       <c r="E57" s="6">
@@ -1811,7 +1805,7 @@
         <v>40146</v>
       </c>
       <c r="C58" s="5" t="s">
-        <v>25</v>
+        <v>17</v>
       </c>
       <c r="D58" s="6">
         <v>1600</v>
@@ -1831,7 +1825,7 @@
         <v>40225</v>
       </c>
       <c r="C59" s="5" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="D59" s="6">
         <v>100</v>
@@ -1871,7 +1865,7 @@
         <v>40375</v>
       </c>
       <c r="C61" s="5" t="s">
-        <v>21</v>
+        <v>11</v>
       </c>
       <c r="D61" s="6">
         <v>100</v>
@@ -1914,7 +1908,7 @@
         <v>40523</v>
       </c>
       <c r="C63" s="5" t="s">
-        <v>46</v>
+        <v>37</v>
       </c>
       <c r="D63" s="6">
         <v>45.22</v>
@@ -1937,7 +1931,7 @@
         <v>40610</v>
       </c>
       <c r="C64" s="5" t="s">
-        <v>23</v>
+        <v>50</v>
       </c>
       <c r="D64" s="6">
         <v>160.03</v>
@@ -1957,7 +1951,7 @@
         <v>40682</v>
       </c>
       <c r="C65" s="5" t="s">
-        <v>34</v>
+        <v>25</v>
       </c>
       <c r="D65" s="6"/>
       <c r="E65" s="6">
@@ -1980,7 +1974,7 @@
         <v>40700</v>
       </c>
       <c r="C66" s="5" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="D66" s="6">
         <v>1600</v>
@@ -2003,7 +1997,7 @@
         <v>40773</v>
       </c>
       <c r="C67" s="5" t="s">
-        <v>24</v>
+        <v>16</v>
       </c>
       <c r="D67" s="6">
         <v>13.76</v>
@@ -2026,7 +2020,7 @@
         <v>40860</v>
       </c>
       <c r="C68" s="5" t="s">
-        <v>19</v>
+        <v>52</v>
       </c>
       <c r="D68" s="6">
         <v>41.28</v>
@@ -2049,7 +2043,7 @@
         <v>40943</v>
       </c>
       <c r="C69" s="5" t="s">
-        <v>20</v>
+        <v>48</v>
       </c>
       <c r="D69" s="6">
         <v>81.33</v>
@@ -2069,7 +2063,7 @@
         <v>41020</v>
       </c>
       <c r="C70" s="5" t="s">
-        <v>34</v>
+        <v>25</v>
       </c>
       <c r="D70" s="6"/>
       <c r="E70" s="6">
@@ -2092,7 +2086,7 @@
         <v>41112</v>
       </c>
       <c r="C71" s="5" t="s">
-        <v>41</v>
+        <v>32</v>
       </c>
       <c r="D71" s="6">
         <v>582.41999999999996</v>
@@ -2115,7 +2109,7 @@
         <v>41195</v>
       </c>
       <c r="C72" s="5" t="s">
-        <v>46</v>
+        <v>37</v>
       </c>
       <c r="D72" s="6">
         <v>50.47</v>
@@ -2135,7 +2129,7 @@
         <v>41199</v>
       </c>
       <c r="C73" s="5" t="s">
-        <v>34</v>
+        <v>25</v>
       </c>
       <c r="D73" s="6"/>
       <c r="E73" s="6">
@@ -2155,7 +2149,7 @@
         <v>41224</v>
       </c>
       <c r="C74" s="5" t="s">
-        <v>52</v>
+        <v>43</v>
       </c>
       <c r="D74" s="6">
         <v>3000</v>
@@ -2175,7 +2169,7 @@
         <v>41309</v>
       </c>
       <c r="C75" s="5" t="s">
-        <v>16</v>
+        <v>49</v>
       </c>
       <c r="D75" s="6">
         <v>69.989999999999995</v>
@@ -2198,7 +2192,7 @@
         <v>41412</v>
       </c>
       <c r="C76" s="5" t="s">
-        <v>43</v>
+        <v>34</v>
       </c>
       <c r="D76" s="6">
         <v>331.07</v>
@@ -2221,7 +2215,7 @@
         <v>41498</v>
       </c>
       <c r="C77" s="7" t="s">
-        <v>18</v>
+        <v>37</v>
       </c>
       <c r="D77" s="6">
         <v>79.459999999999994</v>
@@ -2241,7 +2235,7 @@
         <v>41526</v>
       </c>
       <c r="C78" s="7" t="s">
-        <v>34</v>
+        <v>25</v>
       </c>
       <c r="D78" s="6"/>
       <c r="E78" s="6">
@@ -2261,7 +2255,7 @@
         <v>41600</v>
       </c>
       <c r="C79" s="7" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="D79" s="6">
         <v>100</v>
@@ -2281,7 +2275,7 @@
         <v>41600</v>
       </c>
       <c r="C80" s="7" t="s">
-        <v>22</v>
+        <v>15</v>
       </c>
       <c r="D80" s="6">
         <v>5</v>
@@ -2301,7 +2295,7 @@
         <v>41640</v>
       </c>
       <c r="C81" s="7" t="s">
-        <v>53</v>
+        <v>44</v>
       </c>
       <c r="D81" s="6">
         <v>500</v>
@@ -2344,7 +2338,7 @@
         <v>41794</v>
       </c>
       <c r="C83" s="7" t="s">
-        <v>20</v>
+        <v>48</v>
       </c>
       <c r="D83" s="6">
         <v>81.489999999999995</v>
@@ -2367,7 +2361,7 @@
         <v>41893</v>
       </c>
       <c r="C84" s="5" t="s">
-        <v>48</v>
+        <v>39</v>
       </c>
       <c r="D84" s="6">
         <v>100</v>
@@ -2390,7 +2384,7 @@
         <v>42008</v>
       </c>
       <c r="C85" s="5" t="s">
-        <v>20</v>
+        <v>48</v>
       </c>
       <c r="D85" s="6">
         <v>81.89</v>
@@ -2410,7 +2404,7 @@
         <v>42111</v>
       </c>
       <c r="C86" s="5" t="s">
-        <v>27</v>
+        <v>19</v>
       </c>
       <c r="D86" s="6"/>
       <c r="E86" s="6">
@@ -2430,7 +2424,7 @@
         <v>42220</v>
       </c>
       <c r="C87" s="5" t="s">
-        <v>29</v>
+        <v>47</v>
       </c>
       <c r="D87" s="6">
         <v>200</v>
@@ -2453,7 +2447,7 @@
         <v>42303</v>
       </c>
       <c r="C88" s="5" t="s">
-        <v>48</v>
+        <v>39</v>
       </c>
       <c r="D88" s="6">
         <v>105</v>
@@ -2473,7 +2467,7 @@
         <v>42430</v>
       </c>
       <c r="C89" s="5" t="s">
-        <v>26</v>
+        <v>18</v>
       </c>
       <c r="D89" s="6">
         <v>63</v>
@@ -2496,7 +2490,7 @@
         <v>42537</v>
       </c>
       <c r="C90" s="5" t="s">
-        <v>55</v>
+        <v>46</v>
       </c>
       <c r="D90" s="6">
         <v>25.79</v>
@@ -2516,7 +2510,7 @@
         <v>42646</v>
       </c>
       <c r="C91" s="5" t="s">
-        <v>35</v>
+        <v>26</v>
       </c>
       <c r="D91" s="6">
         <v>65.430000000000007</v>
@@ -2536,7 +2530,7 @@
         <v>42718</v>
       </c>
       <c r="C92" s="5" t="s">
-        <v>34</v>
+        <v>25</v>
       </c>
       <c r="D92" s="6"/>
       <c r="E92" s="6">
@@ -2559,7 +2553,7 @@
         <v>42788</v>
       </c>
       <c r="C93" s="5" t="s">
-        <v>41</v>
+        <v>32</v>
       </c>
       <c r="D93" s="6">
         <v>1186.94</v>
@@ -2582,7 +2576,7 @@
         <v>42911</v>
       </c>
       <c r="C94" s="5" t="s">
-        <v>48</v>
+        <v>39</v>
       </c>
       <c r="D94" s="6">
         <v>115</v>
@@ -2602,7 +2596,7 @@
         <v>43031</v>
       </c>
       <c r="C95" s="5" t="s">
-        <v>30</v>
+        <v>21</v>
       </c>
       <c r="D95" s="6">
         <v>25</v>
@@ -2625,7 +2619,7 @@
         <v>43178</v>
       </c>
       <c r="C96" s="5" t="s">
-        <v>55</v>
+        <v>46</v>
       </c>
       <c r="D96" s="6">
         <v>67.88</v>
@@ -2645,7 +2639,7 @@
         <v>43329</v>
       </c>
       <c r="C97" s="5" t="s">
-        <v>34</v>
+        <v>25</v>
       </c>
       <c r="D97" s="6"/>
       <c r="E97" s="6">
@@ -2668,7 +2662,7 @@
         <v>43483</v>
       </c>
       <c r="C98" s="5" t="s">
-        <v>55</v>
+        <v>46</v>
       </c>
       <c r="D98" s="6">
         <v>76.37</v>
@@ -2688,7 +2682,7 @@
         <v>43582</v>
       </c>
       <c r="C99" s="5" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="D99" s="6">
         <v>25</v>
@@ -2708,7 +2702,7 @@
         <v>43619</v>
       </c>
       <c r="C100" s="5" t="s">
-        <v>35</v>
+        <v>26</v>
       </c>
       <c r="D100" s="6">
         <v>103.99</v>
@@ -2731,7 +2725,7 @@
         <v>43751</v>
       </c>
       <c r="C101" s="5" t="s">
-        <v>47</v>
+        <v>38</v>
       </c>
       <c r="D101" s="6">
         <v>100</v>
@@ -2751,7 +2745,7 @@
         <v>43503</v>
       </c>
       <c r="C102" s="5" t="s">
-        <v>54</v>
+        <v>45</v>
       </c>
       <c r="D102" s="6">
         <v>198.67</v>
@@ -2771,7 +2765,7 @@
         <v>43891</v>
       </c>
       <c r="C103" s="5" t="s">
-        <v>31</v>
+        <v>22</v>
       </c>
       <c r="D103" s="6">
         <v>500</v>
@@ -2794,7 +2788,7 @@
         <v>44002</v>
       </c>
       <c r="C104" s="5" t="s">
-        <v>47</v>
+        <v>38</v>
       </c>
       <c r="D104" s="6">
         <v>110</v>
@@ -2814,7 +2808,7 @@
         <v>44042</v>
       </c>
       <c r="C105" s="5" t="s">
-        <v>50</v>
+        <v>41</v>
       </c>
       <c r="D105" s="6"/>
       <c r="E105" s="6">

</xml_diff>